<commit_message>
Corrected scatter_plot cases description
</commit_message>
<xml_diff>
--- a/doc/aesthetics_scatter.xlsx
+++ b/doc/aesthetics_scatter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC9FA10-8EDE-4FF8-9D71-C0D70A5C72F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9424C22-6819-4775-B693-0A02BFE4FB64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="19">
   <si>
     <t>mixture</t>
   </si>
@@ -58,9 +58,6 @@
     <t>plot_per_sit | text</t>
   </si>
   <si>
-    <t>several_sit &amp; (symbol | group)</t>
-  </si>
-  <si>
     <t>situation</t>
   </si>
   <si>
@@ -68,6 +65,18 @@
   </si>
   <si>
     <t>mixture + version + several_sit &amp; (symbol | group)</t>
+  </si>
+  <si>
+    <t>several_sit</t>
+  </si>
+  <si>
+    <t>all_situations $ shape_sit==none</t>
+  </si>
+  <si>
+    <t>(!all_situations &amp; !successive) | shape_sit == [txt | none]</t>
+  </si>
+  <si>
+    <t>(all_situations | successive) &amp; (shape_sit == [symbol | group])</t>
   </si>
 </sst>
 </file>
@@ -232,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -262,20 +271,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,21 +285,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -314,6 +306,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,47 +613,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.77734375" customWidth="1"/>
+    <col min="15" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.21875" customWidth="1"/>
+    <col min="19" max="22" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="16"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="48"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
@@ -683,64 +722,88 @@
       <c r="R2" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="S2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="23" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="23" t="s">
+      <c r="L3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="22" t="s">
+      <c r="P3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="53"/>
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="35"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="10" t="s">
         <v>8</v>
       </c>
@@ -765,58 +828,82 @@
       <c r="R4" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="S4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="22" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="53"/>
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
@@ -829,10 +916,10 @@
       <c r="J6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="35"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="6" t="s">
         <v>9</v>
       </c>
@@ -845,140 +932,184 @@
       <c r="R6" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="S6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="32" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="33"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="35"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="50"/>
+      <c r="B8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="38"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="50"/>
+      <c r="B10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="42"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="45"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="19" t="s">
+      <c r="E12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -994,11 +1125,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1014,9 +1145,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="50"/>
+      <c r="B15" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1033,7 +1164,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="S1:V1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A14:A15"/>

</xml_diff>

<commit_message>
Updated description of scatter plot tests
</commit_message>
<xml_diff>
--- a/doc/aesthetics_scatter.xlsx
+++ b/doc/aesthetics_scatter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216FA762-446A-48F9-B192-E0B54EC60CAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6504D33F-569B-40A9-B514-240471F65986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>situation</t>
   </si>
   <si>
-    <t>mixture + version + plot_per_sit | text</t>
-  </si>
-  <si>
     <t>mixture + version + several_sit &amp; (symbol | group)</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>attributes defined in version lines (that correspond to aesth$version) should be retrieved in plot$sit$layers[[*]]$mapping</t>
+  </si>
+  <si>
+    <t>mixture + version + plot_per_sit | text | none</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,13 +648,13 @@
       <c r="I1" s="44"/>
       <c r="J1" s="45"/>
       <c r="K1" s="43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="45"/>
       <c r="O1" s="43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P1" s="44"/>
       <c r="Q1" s="44"/>
@@ -888,7 +888,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>2</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>2</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>2</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>2</v>
@@ -1088,12 +1088,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test description matrix
</commit_message>
<xml_diff>
--- a/doc/aesthetics_scatter.xlsx
+++ b/doc/aesthetics_scatter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6504D33F-569B-40A9-B514-240471F65986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DAC0C0-4201-49D0-B754-56BAA80BDD55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="20">
   <si>
     <t>mixture</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>mixture + version + plot_per_sit | text | none</t>
+  </si>
+  <si>
+    <t>if group set to NULL, test group=="group" (ggplot2 default?)</t>
+  </si>
+  <si>
+    <t>WARNING: if all_situation=FALSE and shape_sit!=none, then all_situation is automatically set to TRUE !!!</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,6 @@
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -302,6 +307,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -326,7 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,13 +613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,465 +641,475 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="43" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="43" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="43" t="s">
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="23" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="18" t="s">
+      <c r="L3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="Q3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="20"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="48"/>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="25"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="48"/>
+      <c r="B10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="23"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="47"/>
-      <c r="B8" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="N8" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8" s="24"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="26"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
-      <c r="B10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>11</v>
+      <c r="E12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="48"/>
+      <c r="B15" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>8</v>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="42" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="42" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1110,5 +1126,6 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>